<commit_message>
Aggregated variables but new delivery variables must be converted to TAF!
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v2.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v2.xlsx
@@ -105,9 +105,6 @@
     <t>D8</t>
   </si>
   <si>
-    <t>E177</t>
-  </si>
-  <si>
     <t>Model_Files</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>coeqwal_cs3_scenario_listing_v4.xlsx</t>
+  </si>
+  <si>
+    <t>E178</t>
   </si>
 </sst>
 </file>
@@ -493,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,7 +531,7 @@
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -553,7 +553,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -567,7 +567,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -581,7 +581,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -595,7 +595,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -609,7 +609,7 @@
         <v>24</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -625,15 +625,15 @@
         <v>25</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -641,37 +641,37 @@
         <v>26</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
modified initialization file 030725
</commit_message>
<xml_diff>
--- a/notebooks/CalSim3DataExtractionInitFile_v2.xlsx
+++ b/notebooks/CalSim3DataExtractionInitFile_v2.xlsx
@@ -153,7 +153,7 @@
     <t>coeqwal_cs3_scenario_listing_v4.xlsx</t>
   </si>
   <si>
-    <t>E180</t>
+    <t>E179</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>